<commit_message>
Update OWF Excel file names
</commit_message>
<xml_diff>
--- a/3_Data/ElexonData/ElexonOWFList.xlsx
+++ b/3_Data/ElexonData/ElexonOWFList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cege\Dropbox\David_PostDoc\2_Working\5. LCOE_Model\2_BayesianCFac\ElexonData\ElexonProduction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cege\Dropbox\David_PostDoc\2_Working\5. LCOE_Model\2_BayesianCFac\7_Github\3_Data\ElexonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35863FE-CCA5-414E-809B-DE06877BEDC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0BA0FE-0157-493D-8EB6-D8345489CBEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12585" windowHeight="8730" xr2:uid="{BA3E4129-B6BB-4C64-8A5E-1120A25E1C63}"/>
   </bookViews>

</xml_diff>